<commit_message>
finishing debbuging, and optimizing input_step for GPU
</commit_message>
<xml_diff>
--- a/resources/perf.xlsx
+++ b/resources/perf.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scalian-my.sharepoint.com/personal/remi_cazoulat_scalian_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remi.cazoulat\Documents\GitHub\FluidSim\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6F19819-93A9-468A-8C4B-D187F9EFC6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9000B96-DE74-4972-B808-9FE46854C4B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" xr2:uid="{F49C74B9-8855-4CAB-85AA-9E1768B3CC2F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>res</t>
   </si>
@@ -53,10 +53,34 @@
     <t>OpenGL</t>
   </si>
   <si>
-    <t>inverse</t>
-  </si>
-  <si>
     <t>Vulkan</t>
+  </si>
+  <si>
+    <t>1 (128 x 72)</t>
+  </si>
+  <si>
+    <t>2 (256 * 144)</t>
+  </si>
+  <si>
+    <t>4 (512 * 288)</t>
+  </si>
+  <si>
+    <t>8 (1024 * 576)</t>
+  </si>
+  <si>
+    <t>16 (2048 * 1152)</t>
+  </si>
+  <si>
+    <t>inverse matrix</t>
+  </si>
+  <si>
+    <t>spec :</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>type :</t>
   </si>
 </sst>
 </file>
@@ -118,12 +142,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -134,8 +152,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -205,7 +229,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -219,7 +271,7 @@
       <left style="thick">
         <color indexed="64"/>
       </left>
-      <right style="thick">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -229,41 +281,30 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
+      <bottom style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
+      <top style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
       </bottom>
       <diagonal/>
     </border>
@@ -274,7 +315,9 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color theme="2" tint="-0.24994659260841701"/>
+      </top>
       <bottom style="thick">
         <color indexed="64"/>
       </bottom>
@@ -284,11 +327,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -296,17 +336,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -318,31 +357,43 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -679,267 +730,284 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0488E991-D530-4D10-8C3E-3C7AD5C53B6A}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="9" max="10" width="11.07421875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="32.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="7"/>
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:17" ht="32.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="5"/>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+    </row>
+    <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1">
+      <c r="B3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1">
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1">
-        <v>8</v>
-      </c>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1">
-        <v>16</v>
-      </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="G3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="J3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="K3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="M3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="4" t="s">
+      <c r="N3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="P3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" s="4" t="s">
+      <c r="Q3" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A4" s="6">
+        <v>25</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="17"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A5" s="6">
+        <v>50</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="20"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A6" s="6">
+        <v>75</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="20"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A7" s="6">
+        <v>100</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="20"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A8" s="6">
+        <v>125</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="20"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A9" s="6">
+        <v>150</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="20"/>
+    </row>
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="23"/>
+    </row>
+    <row r="11" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A4" s="8">
-        <v>25</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="20"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A5" s="8">
-        <v>50</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="20"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A6" s="8">
-        <v>75</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="20"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A7" s="8">
-        <v>100</v>
-      </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="20"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A8" s="8">
-        <v>125</v>
-      </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="20"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A9" s="8">
-        <v>150</v>
-      </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="20"/>
-    </row>
-    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="21"/>
-    </row>
-    <row r="11" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>